<commit_message>
Add Steady State Concentration to Flux Test
</commit_message>
<xml_diff>
--- a/flux_test/data_collection.xlsx
+++ b/flux_test/data_collection.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lscheer/git/co2_flux_summer_24/flux_test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\lincoln_scheer\git\co2_flux_summer_24\flux_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F5093B-9055-AA40-A2E6-51BCAB4B0557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF7FAD2-F1BF-49F6-BB02-329BD664FE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{80C4E468-50E1-F042-A9C8-3415909E48ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{80C4E468-50E1-F042-A9C8-3415909E48ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -91,7 +92,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -193,10 +194,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,7 +224,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{1CA424B9-639F-46DD-9777-7AF837918C34}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -237,9 +239,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -277,7 +279,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -383,7 +385,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -525,7 +527,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -533,45 +535,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD0A646-6A95-7746-9FA3-B750A09E3A25}">
-  <dimension ref="C4:H15"/>
+  <dimension ref="C4:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C4" s="4" t="s">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C5" s="5" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -591,7 +593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
@@ -611,7 +613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
@@ -631,150 +633,155 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="2" t="s">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>500</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G9" s="1">
         <v>378</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C10" s="2" t="s">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>527</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="1">
         <v>512</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="2" t="s">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="1">
         <f>(D10-D9)-D8</f>
         <v>4</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="1">
         <f>(G10-G9)-G8</f>
         <v>89</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="2" t="s">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>45432.422222222223</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>45432.445833333331</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="2" t="s">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>45432.433333333334</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>45433.459027777775</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C14" s="2" t="s">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <f>D12-TIME(0,3,0)</f>
         <v>45432.420138888891</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <f>G12-TIME(0,3,0)</f>
         <v>45432.443749999999</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C15" s="2" t="s">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <f>D13-TIME(0,3,0)</f>
         <v>45432.431250000001</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <f>G13-TIME(0,3,0)</f>
         <v>45433.456944444442</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Scripts - After 3003 ppm Flux Test
</commit_message>
<xml_diff>
--- a/flux_test/data_collection.xlsx
+++ b/flux_test/data_collection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\lincoln_scheer\git\co2_flux_summer_24\flux_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lscheer/git/co2_flux_summer_24/flux_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF7FAD2-F1BF-49F6-BB02-329BD664FE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC9C8CB-5848-CB43-BEBC-9037B11BE35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{80C4E468-50E1-F042-A9C8-3415909E48ED}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{80C4E468-50E1-F042-A9C8-3415909E48ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="23">
   <si>
     <t>Low Test</t>
   </si>
@@ -87,6 +86,24 @@
   </si>
   <si>
     <t>Flux Test w/ 400 ppm &amp; 2.5 LPM MFC</t>
+  </si>
+  <si>
+    <t>Flux Test w/ 3003 ppm &amp; 0.2 LPM MFC</t>
+  </si>
+  <si>
+    <t>Ambient Reference Time</t>
+  </si>
+  <si>
+    <t>MFC Rate</t>
+  </si>
+  <si>
+    <t>lpm</t>
+  </si>
+  <si>
+    <t>Steady State Offset</t>
+  </si>
+  <si>
+    <t>Flux Test w/ 3003 ppm &amp; 2.5 LPM MFC</t>
   </si>
 </sst>
 </file>
@@ -110,7 +127,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,6 +143,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -194,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -219,6 +242,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -239,9 +284,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +324,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +430,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +572,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -535,23 +580,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD0A646-6A95-7746-9FA3-B750A09E3A25}">
-  <dimension ref="C4:K28"/>
+  <dimension ref="C4:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
@@ -561,7 +606,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
@@ -573,7 +618,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -593,7 +638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
@@ -613,7 +658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
@@ -633,7 +678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -653,7 +698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
@@ -673,7 +718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
@@ -695,7 +740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
@@ -715,7 +760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
@@ -735,7 +780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
@@ -757,7 +802,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
@@ -779,19 +824,632 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K28">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C21" s="13" t="s">
         <v>2</v>
       </c>
+      <c r="D21" s="13">
+        <v>0.64180000000000004</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C22" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C23" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="13">
+        <v>30.030100000000001</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C24" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="13">
+        <v>558</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C25" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="14">
+        <v>45433.489583333336</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C26" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="13">
+        <v>536</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <f>D26+D23</f>
+        <v>566.03009999999995</v>
+      </c>
+      <c r="G26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C27" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="14">
+        <v>45433.490972222222</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C28" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="14">
+        <v>45433.507638888892</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C29" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="14">
+        <f>D27-TIME(0,3,0)</f>
+        <v>45433.488888888889</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C30" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="14">
+        <f>D28-TIME(0,3,0)</f>
+        <v>45433.505555555559</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="E32" s="12"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C33" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="13">
+        <v>3.2088000000000001</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C34" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C35" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="13">
+        <v>150.15029999999999</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C36" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="13">
+        <v>648</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C37" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="14">
+        <v>45433.518750000003</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C38" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="13">
+        <v>545</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <f>D38+D35</f>
+        <v>695.15030000000002</v>
+      </c>
+      <c r="G38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C39" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="14">
+        <v>45433.519444444442</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C40" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="14">
+        <v>45433.536805555559</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C41" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="14">
+        <f>D39-TIME(0,3,0)</f>
+        <v>45433.517361111109</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C42" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="14">
+        <f>D40-TIME(0,3,0)</f>
+        <v>45433.534722222226</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C44" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="11"/>
+      <c r="E44" s="12"/>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C45" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="13">
+        <v>5.7759</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C46" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="13">
+        <v>0.18</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C47" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="13">
+        <v>270.2706</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C48" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="13">
+        <v>737</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C49" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="14">
+        <v>45433.570138888892</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C50" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="13">
+        <v>548</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <f>D50+D47</f>
+        <v>818.27060000000006</v>
+      </c>
+      <c r="G50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C51" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="14">
+        <v>45433.552777777775</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C52" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="14">
+        <v>45433.570138888892</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C53" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="14">
+        <f>D51-TIME(0,3,0)</f>
+        <v>45433.550694444442</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C54" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="14">
+        <f>D52-TIME(0,3,0)</f>
+        <v>45433.568055555559</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C56" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="16"/>
+      <c r="E56" s="17"/>
+    </row>
+    <row r="57" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C57" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="18">
+        <v>8.0221</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C58" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C59" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" s="18">
+        <v>375.3759</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C60" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C61" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="19"/>
+      <c r="E61" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C62" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F62">
+        <f>D62+D59</f>
+        <v>375.3759</v>
+      </c>
+      <c r="G62" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C63" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" s="19"/>
+      <c r="E63" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C64" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="19"/>
+      <c r="E64" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C65" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="19">
+        <f>D63-TIME(0,3,0)</f>
+        <v>-2.0833333333333333E-3</v>
+      </c>
+      <c r="E65" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C66" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="19">
+        <f>D64-TIME(0,3,0)</f>
+        <v>-2.0833333333333333E-3</v>
+      </c>
+      <c r="E66" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C68" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D68" s="16"/>
+      <c r="E68" s="17"/>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C69" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" s="18">
+        <v>12.6061</v>
+      </c>
+      <c r="E69" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C70" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D70" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="E70" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C71" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71" s="18">
+        <v>589.87630000000001</v>
+      </c>
+      <c r="E71" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C72" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C73" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" s="19"/>
+      <c r="E73" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C74" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F74">
+        <f>D74+D71</f>
+        <v>589.87630000000001</v>
+      </c>
+      <c r="G74" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C75" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="19"/>
+      <c r="E75" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C76" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="19"/>
+      <c r="E76" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C77" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" s="19">
+        <f>D75-TIME(0,3,0)</f>
+        <v>-2.0833333333333333E-3</v>
+      </c>
+      <c r="E77" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C78" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="19">
+        <f>D76-TIME(0,3,0)</f>
+        <v>-2.0833333333333333E-3</v>
+      </c>
+      <c r="E78" s="18" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C68:E68"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C20:E20"/>
   </mergeCells>
   <conditionalFormatting sqref="D11">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -803,7 +1461,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Update Flux Test Data
</commit_message>
<xml_diff>
--- a/flux_test/data_collection.xlsx
+++ b/flux_test/data_collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lscheer/git/co2_flux_summer_24/flux_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC9C8CB-5848-CB43-BEBC-9037B11BE35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158C0E66-6905-C04B-9CAF-CE39CEC71FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{80C4E468-50E1-F042-A9C8-3415909E48ED}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="28800" windowHeight="17540" xr2:uid="{80C4E468-50E1-F042-A9C8-3415909E48ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="24">
   <si>
     <t>Low Test</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Flux Test w/ 3003 ppm &amp; 2.5 LPM MFC</t>
+  </si>
+  <si>
+    <t>Observed Steady State Offset</t>
   </si>
 </sst>
 </file>
@@ -217,10 +220,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -242,28 +258,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,43 +578,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD0A646-6A95-7746-9FA3-B750A09E3A25}">
-  <dimension ref="C4:K78"/>
+  <dimension ref="C4:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
@@ -825,628 +826,565 @@
       </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="3">
         <v>0.64180000000000004</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="F21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="3">
+        <v>3.2088000000000001</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="3">
+        <v>5.7759</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="3">
         <v>0.02</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="F22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="3">
         <v>30.030100000000001</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="3">
+        <v>150.15029999999999</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="3">
+        <v>270.2706</v>
+      </c>
+      <c r="K23" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="3">
         <v>558</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="3">
+        <v>648</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" s="3">
+        <v>737</v>
+      </c>
+      <c r="K24" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="4">
         <v>45433.489583333336</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="4">
+        <v>45433.518750000003</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="4">
+        <v>45433.570138888892</v>
+      </c>
+      <c r="K25" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="3">
         <v>536</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26">
-        <f>D26+D23</f>
-        <v>566.03009999999995</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="E26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="3">
+        <v>545</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="3">
+        <v>548</v>
+      </c>
+      <c r="K26" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="4">
         <v>45433.490972222222</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="K27">
-        <v>2</v>
+      <c r="E27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="4">
+        <v>45433.519444444442</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="4">
+        <v>45433.552777777775</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="4">
         <v>45433.507638888892</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="4">
+        <v>45433.536805555559</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" s="4">
+        <v>45433.570138888892</v>
+      </c>
+      <c r="K28" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="4">
         <f>D27-TIME(0,3,0)</f>
         <v>45433.488888888889</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E29" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="4">
+        <f>G27-TIME(0,3,0)</f>
+        <v>45433.517361111109</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="4">
+        <f>J27-TIME(0,3,0)</f>
+        <v>45433.550694444442</v>
+      </c>
+      <c r="K29" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="4">
         <f>D28-TIME(0,3,0)</f>
         <v>45433.505555555559</v>
       </c>
-      <c r="E30" s="13" t="s">
-        <v>13</v>
+      <c r="E30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="4">
+        <f>G28-TIME(0,3,0)</f>
+        <v>45433.534722222226</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="4">
+        <f>J28-TIME(0,3,0)</f>
+        <v>45433.568055555559</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="18">
+        <f>D24-D26</f>
+        <v>22</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="18">
+        <f>G24-G26</f>
+        <v>103</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" s="18">
+        <f>J24-J26</f>
+        <v>189</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="12"/>
-    </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C33" s="13" t="s">
+      <c r="C32" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="9"/>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C33" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="13">
-        <v>3.2088000000000001</v>
-      </c>
-      <c r="E33" s="13" t="s">
+      <c r="D33" s="5">
+        <v>8.0221</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C34" s="13" t="s">
+      <c r="F33" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G33" s="5">
+        <v>12.6061</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C34" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E34" s="13" t="s">
+      <c r="D34" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C35" s="13" t="s">
+      <c r="F34" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C35" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="13">
-        <v>150.15029999999999</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C36" s="13" t="s">
+      <c r="D35" s="5">
+        <v>375.3759</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" s="5">
+        <v>589.87630000000001</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C36" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="13">
-        <v>648</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C37" s="13" t="s">
+      <c r="D36" s="5"/>
+      <c r="E36" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C37" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="14">
-        <v>45433.518750000003</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C38" s="13" t="s">
+      <c r="D37" s="6"/>
+      <c r="E37" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C38" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D38" s="13">
-        <v>545</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F38">
-        <f>D38+D35</f>
-        <v>695.15030000000002</v>
-      </c>
-      <c r="G38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C39" s="13" t="s">
+      <c r="D38" s="5"/>
+      <c r="E38" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C39" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="14">
-        <v>45433.519444444442</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C40" s="13" t="s">
+      <c r="D39" s="6"/>
+      <c r="E39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="6"/>
+      <c r="H39" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C40" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="14">
-        <v>45433.536805555559</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C41" s="13" t="s">
+      <c r="D40" s="6"/>
+      <c r="E40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C41" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="14">
+      <c r="D41" s="6">
         <f>D39-TIME(0,3,0)</f>
-        <v>45433.517361111109</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C42" s="13" t="s">
+        <v>-2.0833333333333333E-3</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="6">
+        <f>G39-TIME(0,3,0)</f>
+        <v>-2.0833333333333333E-3</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C42" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D42" s="14">
+      <c r="D42" s="6">
         <f>D40-TIME(0,3,0)</f>
-        <v>45433.534722222226</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C44" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="12"/>
-    </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C45" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D45" s="13">
-        <v>5.7759</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C46" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46" s="13">
-        <v>0.18</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C47" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D47" s="13">
-        <v>270.2706</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C48" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="13">
-        <v>737</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C49" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D49" s="14">
-        <v>45433.570138888892</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C50" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="13">
-        <v>548</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>4</v>
-      </c>
+        <v>-2.0833333333333333E-3</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="6">
+        <f>G40-TIME(0,3,0)</f>
+        <v>-2.0833333333333333E-3</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F50">
-        <f>D50+D47</f>
-        <v>818.27060000000006</v>
+        <f>G38+G35</f>
+        <v>589.87630000000001</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C51" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" s="14">
-        <v>45433.552777777775</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C52" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="14">
-        <v>45433.570138888892</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C53" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D53" s="14">
-        <f>D51-TIME(0,3,0)</f>
-        <v>45433.550694444442</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C54" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D54" s="14">
-        <f>D52-TIME(0,3,0)</f>
-        <v>45433.568055555559</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C56" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" s="16"/>
-      <c r="E56" s="17"/>
-    </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C57" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D57" s="18">
-        <v>8.0221</v>
-      </c>
-      <c r="E57" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C58" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D58" s="18">
-        <v>2.5</v>
-      </c>
-      <c r="E58" s="18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C59" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D59" s="18">
-        <v>375.3759</v>
-      </c>
-      <c r="E59" s="18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C60" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C61" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D61" s="19"/>
-      <c r="E61" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C62" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F62">
-        <f>D62+D59</f>
-        <v>375.3759</v>
-      </c>
-      <c r="G62" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C63" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D63" s="19"/>
-      <c r="E63" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C64" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D64" s="19"/>
-      <c r="E64" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C65" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D65" s="19">
-        <f>D63-TIME(0,3,0)</f>
-        <v>-2.0833333333333333E-3</v>
-      </c>
-      <c r="E65" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C66" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D66" s="19">
-        <f>D64-TIME(0,3,0)</f>
-        <v>-2.0833333333333333E-3</v>
-      </c>
-      <c r="E66" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C68" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D68" s="16"/>
-      <c r="E68" s="17"/>
-    </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C69" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D69" s="18">
-        <v>12.6061</v>
-      </c>
-      <c r="E69" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C70" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D70" s="18">
-        <v>2.5</v>
-      </c>
-      <c r="E70" s="18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C71" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D71" s="18">
-        <v>589.87630000000001</v>
-      </c>
-      <c r="E71" s="18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C72" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C73" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D73" s="19"/>
-      <c r="E73" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C74" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F74">
-        <f>D74+D71</f>
-        <v>589.87630000000001</v>
-      </c>
-      <c r="G74" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C75" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D75" s="19"/>
-      <c r="E75" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C76" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D76" s="19"/>
-      <c r="E76" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C77" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D77" s="19">
-        <f>D75-TIME(0,3,0)</f>
-        <v>-2.0833333333333333E-3</v>
-      </c>
-      <c r="E77" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C78" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D78" s="19">
-        <f>D76-TIME(0,3,0)</f>
-        <v>-2.0833333333333333E-3</v>
-      </c>
-      <c r="E78" s="18" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="I20:K20"/>
     <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="F32:H32"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:H20"/>
   </mergeCells>
   <conditionalFormatting sqref="D11">
     <cfRule type="colorScale" priority="4">

</xml_diff>